<commit_message>
Display completed, Testing to be done!
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\darshil\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D33202-9B39-4907-B950-E3555005FE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,139 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>ufile abc.txt ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile abc.c ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile s.pdf ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile abc.c ~/spdf/test</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/abc.c</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/abc.txt</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/s.pdf</t>
+  </si>
+  <si>
+    <t>ufile a.c ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile a.pdf ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile a.txt ~/smain/test</t>
+  </si>
+  <si>
+    <t>ufile s.pdf ~/spdf/test</t>
+  </si>
+  <si>
+    <t>ufile s.pdf ~/stext/test</t>
+  </si>
+  <si>
+    <t>ufile s.pptx ~/smain/test</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/a.txt</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/s234.pdf</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/s234.c</t>
+  </si>
+  <si>
+    <t>rmfile ~/smain/test/s.pptx</t>
+  </si>
+  <si>
+    <t>rmfile ~/spdf/test/s.pdf</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/def.c</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/def.txt</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/def.pdf</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/def.pptx</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/de.c</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/de.txt</t>
+  </si>
+  <si>
+    <t>dfile ~/smain/test/de.pdf</t>
+  </si>
+  <si>
+    <t>dfile ~/spdf/test/de.txt</t>
+  </si>
+  <si>
+    <t>dfile ~/stxt/test/de.txt</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>abc.txt</t>
+  </si>
+  <si>
+    <t>abc.c</t>
+  </si>
+  <si>
+    <t>s.pdf</t>
+  </si>
+  <si>
+    <t>in PWD</t>
+  </si>
+  <si>
+    <t>in server</t>
+  </si>
+  <si>
+    <t>def.c</t>
+  </si>
+  <si>
+    <t>def.txt</t>
+  </si>
+  <si>
+    <t>def.pdf</t>
+  </si>
+  <si>
+    <t>display ~/smain/spdf.abc.c</t>
+  </si>
+  <si>
+    <t>display ~/spdf/</t>
+  </si>
+  <si>
+    <t>display ~/stxt/</t>
+  </si>
+  <si>
+    <t>display ~/smain/test</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +467,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="48.26953125" customWidth="1"/>
+    <col min="2" max="2" width="69.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All command done! Test one final time and check error handling with appropriate message. Also add comments for dtar
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\darshil\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D33202-9B39-4907-B950-E3555005FE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EDF7D4-6FB5-4136-82A3-AD82CB4130ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>pass</t>
   </si>
@@ -141,9 +141,6 @@
     <t>def.pdf</t>
   </si>
   <si>
-    <t>display ~/smain/spdf.abc.c</t>
-  </si>
-  <si>
     <t>display ~/spdf/</t>
   </si>
   <si>
@@ -151,6 +148,63 @@
   </si>
   <si>
     <t>display ~/smain/test</t>
+  </si>
+  <si>
+    <t>in servers</t>
+  </si>
+  <si>
+    <t>display ~/smain/test2</t>
+  </si>
+  <si>
+    <t>test1 in main</t>
+  </si>
+  <si>
+    <t>test2 in pdf and text</t>
+  </si>
+  <si>
+    <t>test 3 in main and pdf</t>
+  </si>
+  <si>
+    <t>test 4 in main and text</t>
+  </si>
+  <si>
+    <t>display ~/smain/test3</t>
+  </si>
+  <si>
+    <t>display ~/smain/test4</t>
+  </si>
+  <si>
+    <t>display ~/smain/test5</t>
+  </si>
+  <si>
+    <t>test5 in none</t>
+  </si>
+  <si>
+    <t>display ~/smain/test6</t>
+  </si>
+  <si>
+    <t>test 6 in all but empty</t>
+  </si>
+  <si>
+    <t>dtar .c</t>
+  </si>
+  <si>
+    <t>dtar .pdf</t>
+  </si>
+  <si>
+    <t>dtar .txt</t>
+  </si>
+  <si>
+    <t>dtar .pptx</t>
+  </si>
+  <si>
+    <t>dtar .xlxs</t>
+  </si>
+  <si>
+    <t>ufile ~/smain/</t>
+  </si>
+  <si>
+    <t>ufile</t>
   </si>
 </sst>
 </file>
@@ -468,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,6 +601,16 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
@@ -615,7 +679,7 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -644,22 +708,79 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>40</v>
+      <c r="C47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>